<commit_message>
large set of changes
</commit_message>
<xml_diff>
--- a/src/data/faq.xlsx
+++ b/src/data/faq.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-26320" yWindow="4980" windowWidth="23040" windowHeight="13720" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="-26920" yWindow="8480" windowWidth="23040" windowHeight="13720" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="faq-tilaus" sheetId="1" r:id="rId1"/>
@@ -92,9 +92,6 @@
     <t>Mikä tämä sivusto on</t>
   </si>
   <si>
-    <t>Ota yhteyttä ja kerro minkälainen projekti on kysessä. Kartoitan projektin työnmäärän ja teen tarjouksen. Tarjoukseen on määritelty aika arvio työvaiheista ja projektin lopullisesta deadlinesta, jos tarpeesi ovat selkeät voimme myös sopia kiinteästä hinnasta.  Tarjouksen pyytäminen ja siinä tapahtuva konsultointi on täysin ilmaista.</t>
-  </si>
-  <si>
     <t>How much does this cost</t>
   </si>
   <si>
@@ -108,10 +105,6 @@
   </si>
   <si>
     <t>How to get started</t>
-  </si>
-  <si>
-    <t>Contact me and tell what kind of project is in question. I'll map the workload of the project and will make you an offer.
-If you have clear needs we can also agree on a fixed price. Requesting the offer is completely free.</t>
   </si>
   <si>
     <t>Usually 2- 3 weeks from idea to functional website. Note that this is influenced by many factors, such as the complexity of the project and the amount of content that is needed. Simple marketing and demo sites can be done in less than a week, and the pages will be completed faster if most of the text and image content is already completed.</t>
@@ -139,12 +132,6 @@
 </t>
   </si>
   <si>
-    <t>I charge 20e/h for the design and about 40e/h coding, depending on what technologies I use. In this case, the simple webpages cost about 200e - 750e and the complete web service is about 1200e - 3000e. If you have a tight budget we can also agree on a fixed price and make the sites hosting cost 0e/month.</t>
-  </si>
-  <si>
-    <t>laskutan 20e/h suunnittelusta ja noin 40e/h koodaamisesta riippuen mitä tekniikoita käytän. Tällöin yksinkertaiset verkkosivut maksavat noin 300e - 750e ja verkkopalvelujen tuottaminen noin 1200e - 3000e. Jos sinulla on tiukka budjetti voimme myös sopia kiinteästä hinnasta ja tehdä sivuston hostaaminen 0e/kk.</t>
-  </si>
-  <si>
     <t>Web suunnittelu</t>
   </si>
   <si>
@@ -155,6 +142,19 @@
   </si>
   <si>
     <t>Tämä on henkilökohtainen verkkosivusto tarkoitettu rekrytointiin ja uusien asiakkaiden hankintaan. Sivusto on tehty käyttäen JAMstack:iä (Gatsby.js) ja hostaan sitä Digitaloceanilla, edessä Cloudfare CDN, joiden avulla se lautautuu salamannopeasti ympärimaailmaa. Ota  yhteyttä jos tarvitset tämän kaltaiset verkkosivut henkilökohtaisen brändin kasvattamiseen.</t>
+  </si>
+  <si>
+    <t>laskutan 17e/h suunnittelusta ja noin 35e/h koodaamisesta riippuen mitä tekniikoita käytän. Tällöin yksinkertaiset verkkosivut maksavat noin 300e - 750e ja verkkopalvelujen tuottaminen noin 1200e - 3000e. Jos sinulla on tiukka budjetti voimme myös sopia kiinteästä hinnasta ja tehdä sivuston hostaaminen 0e/kk.</t>
+  </si>
+  <si>
+    <t>I charge 17e/h for the design and about 30e/h coding, depending on what technologies I use. In this case, the simple webpages cost about 300e - 750e and the complete web service is about 1200e - 3000e. If you have a tight budget we can also agree on a fixed price and make the sites hosting cost 0e/month.</t>
+  </si>
+  <si>
+    <t>Ota yhteyttä ja kerro minkälainen projekti on kysessä. Kartoitan projektin työnmäärän ja teen tarjouksen. Tarjoukseen on määritelty aika arvio työvaiheista ja projektin lopullisesta deadlinesta, jos budjettisi on tiukka voimme myös sopia kiinteästä hinnasta. Tarjouksen pyytäminen ja siinä tapahtuva konsultointi on täysin ilmaista.</t>
+  </si>
+  <si>
+    <t>Contact me and tell what kind of project is in question. I'll map the workload of the project and will make you an offer.
+If you budget is tight we can also agree on a fixed price. Requesting the offer is completely free.</t>
   </si>
 </sst>
 </file>
@@ -528,7 +528,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView zoomScale="135" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -549,7 +549,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -557,7 +557,7 @@
         <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -585,8 +585,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -604,34 +604,34 @@
     </row>
     <row r="2" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="20" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -666,7 +666,7 @@
         <v>16</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="20" x14ac:dyDescent="0.2">
@@ -674,15 +674,15 @@
         <v>17</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B4" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -716,18 +716,18 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>28</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="20" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>29</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -745,7 +745,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -764,7 +764,7 @@
         <v>18</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -795,10 +795,10 @@
     </row>
     <row r="2" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>